<commit_message>
update for Week 1
</commit_message>
<xml_diff>
--- a/data/syllabus.xlsx
+++ b/data/syllabus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daviddl\Documents\EDUC\641\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daviddl\Documents\EDUC\EDUC641_22F\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Weeks</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Assignments</t>
-  </si>
-  <si>
-    <t>Quizzes</t>
   </si>
   <si>
     <t>Summarizing and displaying continuous data</t>
@@ -55,21 +52,6 @@
   <si>
     <t xml:space="preserve">
 Assignment 2</t>
-  </si>
-  <si>
-    <t>Quiz 1</t>
-  </si>
-  <si>
-    <t>Quiz 2</t>
-  </si>
-  <si>
-    <t>Quiz 3</t>
-  </si>
-  <si>
-    <t>Quiz 4</t>
-  </si>
-  <si>
-    <t>Quiz 5</t>
   </si>
   <si>
     <t>Final</t>
@@ -107,9 +89,6 @@
     <t>Assignment 3</t>
   </si>
   <si>
-    <t>LSWR Ch 2 and 3 &lt;br&gt; [Clayton 2020](https://nautil.us/issue/92/frontiers/how-eugenics-shaped-statistics)</t>
-  </si>
-  <si>
     <t>LSWR Ch 6 &lt;br&gt; [Evans 2020](https://www.newstatesman.com/uncategorized/2020/07/ra-fisher-and-science-hatred)</t>
   </si>
   <si>
@@ -159,6 +138,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>LSWR Ch 2 and 3 &lt;br&gt; [Clayton 2020](https://nautil.us/how-eugenics-shaped-statistics-238014/)</t>
   </si>
 </sst>
 </file>
@@ -531,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,9 +530,9 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -559,153 +541,129 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update main course with various shifts for 2023
</commit_message>
<xml_diff>
--- a/data/syllabus.xlsx
+++ b/data/syllabus.xlsx
@@ -95,9 +95,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>Intro to scienctific principles and data analysis</t>
-  </si>
-  <si>
     <t>Assignment 1</t>
   </si>
   <si>
@@ -107,18 +104,6 @@
     <t>Assignment 3</t>
   </si>
   <si>
-    <t>LSWR Ch 2 and 3 &lt;br&gt; [Clayton 2020](https://nautil.us/issue/92/frontiers/how-eugenics-shaped-statistics)</t>
-  </si>
-  <si>
-    <t>LSWR Ch 6 &lt;br&gt; [Evans 2020](https://www.newstatesman.com/uncategorized/2020/07/ra-fisher-and-science-hatred)</t>
-  </si>
-  <si>
-    <t>LSWR Ch 11 and 12 &lt;br&gt; [Levy 2019](http://gppreview.com/2019/12/16/eugenics-ethics-statistical-analysis/)</t>
-  </si>
-  <si>
-    <t>LSWR Ch 5 and 10 &lt;br&gt; [Hu 2021](https://bostonreview.net/science-nature-race/lily-hu-race-policing-and-limits-social-science)</t>
-  </si>
-  <si>
     <t>LSWR Ch 15.1-15.2</t>
   </si>
   <si>
@@ -159,6 +144,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Intro to scientific principles and data analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSWR Ch 5 and 10 </t>
+  </si>
+  <si>
+    <t>LSWR Ch 11 and 12 &lt;br&gt; [Evans 2020](https://www.newstatesman.com/uncategorized/2020/07/ra-fisher-and-science-hatred)</t>
+  </si>
+  <si>
+    <t>LSWR Ch 6 &lt;br&gt; [Clayton 2020](https://nautil.us/issue/92/frontiers/how-eugenics-shaped-statistics)</t>
+  </si>
+  <si>
+    <t>LSWR Ch 2 and 3 &lt;br&gt;Light, Singer &amp; Willet 1990, Ch. 2</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,16 +570,16 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -590,19 +590,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -610,16 +610,16 @@
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -630,19 +630,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -650,16 +650,16 @@
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -670,22 +670,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Fix rendering issues with Fall 2023 update
</commit_message>
<xml_diff>
--- a/data/syllabus.xlsx
+++ b/data/syllabus.xlsx
@@ -92,9 +92,6 @@
     <t xml:space="preserve"> -</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Assignment 1</t>
   </si>
   <si>
@@ -158,7 +155,10 @@
     <t>LSWR Ch 6 &lt;br&gt; [Clayton 2020](https://nautil.us/issue/92/frontiers/how-eugenics-shaped-statistics)</t>
   </si>
   <si>
-    <t>LSWR Ch 2 and 3 &lt;br&gt;Light, Singer &amp; Willet 1990, Ch. 2</t>
+    <t>LSWR Ch 2 and 3 &lt;br&gt; Light, Singer &amp; Willet 1990, Ch. 2</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -570,16 +570,16 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -590,19 +590,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -610,16 +610,16 @@
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -630,19 +630,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -650,16 +650,16 @@
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -670,22 +670,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Fix rendering issue in syllabus
</commit_message>
<xml_diff>
--- a/data/syllabus.xlsx
+++ b/data/syllabus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daviddl\Documents\EDUC\641\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daviddl\Documents\EDUC\EDUC641_23F\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -149,16 +149,16 @@
     <t xml:space="preserve">LSWR Ch 5 and 10 </t>
   </si>
   <si>
-    <t>LSWR Ch 11 and 12 &lt;br&gt; [Evans 2020](https://www.newstatesman.com/uncategorized/2020/07/ra-fisher-and-science-hatred)</t>
-  </si>
-  <si>
-    <t>LSWR Ch 6 &lt;br&gt; [Clayton 2020](https://nautil.us/issue/92/frontiers/how-eugenics-shaped-statistics)</t>
-  </si>
-  <si>
-    <t>LSWR Ch 2 and 3 &lt;br&gt; Light, Singer &amp; Willet 1990, Ch. 2</t>
-  </si>
-  <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>LSWR Ch 2 and 3  &lt;br&gt; Light, Singer &amp; Willet 1990, Ch. 2</t>
+  </si>
+  <si>
+    <t>LSWR Ch 6  &lt;br&gt; [Clayton 2020](https://nautil.us/issue/92/frontiers/how-eugenics-shaped-statistics)</t>
+  </si>
+  <si>
+    <t>LSWR Ch 11 and 12  &lt;br&gt; [Evans 2020](https://www.newstatesman.com/uncategorized/2020/07/ra-fisher-and-science-hatred)</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -579,7 +579,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -599,7 +599,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -619,7 +619,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>

</xml_diff>